<commit_message>
merge in look up
I think there is an issue with the merge because not all of the biotic are in the look up table.

Co-Authored-By: Colleen R Miller <73894369+ccm246@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data/data_cleaning/Kyle_RecodeSubflows-Feb102025.xlsx
+++ b/data/data_cleaning/Kyle_RecodeSubflows-Feb102025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylemanley/Documents/Postdoc/BCCA/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/lade8828_colorado_edu/Documents/Documents/GitHub/BCCAch7/data/data_cleaning/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5C0261-C6FE-2749-AFCB-B8FA52DAB5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CB3B8B0B-12C6-9144-ABB9-16B34B0D07BD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17940" xr2:uid="{CB3B8B0B-12C6-9144-ABB9-16B34B0D07BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -933,7 +933,7 @@
   <dimension ref="A1:EB5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -1944,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:132" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:132" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
kyles recoded file fixed dube fixed
</commit_message>
<xml_diff>
--- a/data/data_cleaning/Kyle_RecodeSubflows-Feb102025.xlsx
+++ b/data/data_cleaning/Kyle_RecodeSubflows-Feb102025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/lade8828_colorado_edu/Documents/Documents/GitHub/BCCAch7/data/data_cleaning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basti\Documents\GitHub\BCCAch7\data\data_cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5C0261-C6FE-2749-AFCB-B8FA52DAB5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493BA00C-0B12-4992-80B5-2AD69ACA5117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17940" xr2:uid="{CB3B8B0B-12C6-9144-ABB9-16B34B0D07BD}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{CB3B8B0B-12C6-9144-ABB9-16B34B0D07BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="165">
   <si>
     <t>kyle.manley@colorado.edu</t>
   </si>
@@ -65,38 +65,19 @@
     <t>Sociocultural</t>
   </si>
   <si>
-    <t>Governance, Diplomatic/Financial Aid</t>
-  </si>
-  <si>
-    <t>""Progress in protecting and restoring habitat connectivity has been slow, but ecological corridors are key to maintaining biodiversity and supporting transboundary governance and international collaboration""; ""The first draft of the post-2020 Global Biodiversity Framework provides 21 action-oriented targets for 2030... Most of the framework targets have direct or indirect impacts on climate change mitigation... These include integrating Indigenous and Local Knowledge (ILK) and Indigenous Peoples and Local Communities (IPLCs) in biodiversity conservation strategies""‚Äã.; ""Enhancing efficiency and effectiveness of protected areas in fragmented land- and sea-scapes requires establishment of ecological corridors... Hallmarks of successful connectivity conservation include community involvement, habitat priority setting, restoration actions, and environmental services payments that satisfy tenets of climate-smart conservation and improve the resilience of human and ecological communities""‚Äã.; ""Improving the linkages between the different scales of actions is essential for successfully implementing joint biodiversity and climate actions. Locally motivated biodiversity conservation actions can be incentivized, guided and prioritized by international objectives and targets, including climate mitigation and adaptation objectives... Local initiatives matter since the benefits of many small and local biodiversity measures accumulate to make a large contribution to climate mitigation, while also providing multiple local benefits.""; ""Therefore, local to global policies and
-practices designed for biodiversity conservation and climate change
-mitigation should be considered in an integrated and consultative way in mixed-use. land-and sea-scapes so that win-win synergies and nature's contributions to people can be maximized.""</t>
-  </si>
-  <si>
     <t>Climate change (generic), Precipitation directional change, Drought, Sea temperature change, Sea ice area change, Sea level rise, Seawater chemistry, Wildfires, Floods, Hurricanes</t>
   </si>
   <si>
     <t>Alaska; Arctic</t>
   </si>
   <si>
-    <t xml:space="preserve">""The Convention on Biological Diversity (CBD) and the United Nations Framework Convention on Climate Change (UNFCCC) have largely addressed biodiversity and climate challenges separately, despite evidence that conservation actions can simultaneously slow climate change and reduce biodiversity loss""‚Äã; ""Better management of permafrost wetlands, stopping destructive activities (drainage or excavation), preserving undamaged peatlands, rewetting artificially drained areas and restoring degraded areas will help maintain their biodiversity and keep carbon locked in the ground... such management actions have been successfully implemented by the plan on the Long-Term Gravel Pad Reclamation in Alaska""‚Äã; ""In northern high-latitude ecosystems, introducing large herbivores compacts snow and decreases its depth due to winter grazing and animal movements. This substantially reduces the thermal insulation efficiency of snow during wintertime and exposes permafrost to colder temperatures, thereby preventing or decreasing CH4 release from permafrost thawing""‚Äã; ""The adoption of the REDD+ mechanism... has provided a significant opportunity to align national climate change mitigation and biodiversity goals and has strengthened international efforts to slow and ultimately avoid deforestation. Recent evidence shows that REDD+ projects have been effective in some regions, but efforts are not always sustained over the long term and a range of barriers exists""‚Äã‚Äã; ""The post-2020 Global Biodiversity Framework provides 21 action-oriented targets for 2030... These include integrating Indigenous and Local Knowledge (ILK) and Indigenous Peoples and Local Communities (IPLCs) in biodiversity conservation strategies""‚Äã; ""There are high expectations for the upcoming CBD fifteenth Conference of the Parties... to finalize a new set of ambitious actions""; </t>
-  </si>
-  <si>
     <t>Increase</t>
   </si>
   <si>
     <t>Complex change</t>
   </si>
   <si>
-    <t>The paper primarily addresses global governance frameworks (e.g., CBD, UNFCCC) and international mechanisms (e.g., REDD+) for biodiversity and climate action. While the flows themselves are not explicitly North American in origin or direction, these frameworks are directly applicable to:
-Transboundary governance across and between North American countries (NA Countries&lt;-&gt;NA Countries).
-The inclusion of Indigenous and Tribal Nations in these frameworks, which are critical stakeholders within North America (Indigenous&lt;-&gt;NA Countries).</t>
-  </si>
-  <si>
     <t>OTHER - described in above short answer question, specify directionality</t>
-  </si>
-  <si>
-    <t>""The first draft of the post-2020 Global Biodiversity Framework provides 21 action-oriented targets for 2030... These include integrating Indigenous and Local Knowledge (ILK) and Indigenous Peoples and Local Communities (IPLCs) in biodiversity conservation strategies""; ""Enhancing efficiency and effectiveness of protected areas in fragmented land- and sea-scapes requires the establishment of ecological corridors... Hallmarks of successful connectivity conservation include community involvement, habitat priority setting, restoration actions, and environmental services payments""; ""The Convention on Biological Diversity (CBD) and the United Nations Framework Convention on Climate Change (UNFCCC) have largely addressed biodiversity and climate challenges separately, despite evidence that conservation actions can simultaneously slow climate change and reduce biodiversity loss""‚Äã; ""The adoption of the REDD+ mechanism (reducing emissions from deforestation and forest degradation in developing countries) by the UNFCCC in 2007, has provided a significant opportunity to align national climate change mitigation and biodiversity goals and has strengthened international efforts to slow and ultimately avoid deforestation""; ""Recent evidence shows that REDD+ projects have been effective in some regions but efforts are not always sustained over the long term, and a range of barriers exists in other regions""</t>
   </si>
   <si>
     <t>Decrease</t>
@@ -549,9 +530,6 @@
   </si>
   <si>
     <t xml:space="preserve">""The adoption of the REDD+ mechanism (reducing emissions from deforestation and forest degradation in developing countries) by the UNFCCC in 2007, has provided a significant opportunity to align national climate change mitigation and biodiversity goals and has strengthened international efforts to slow and ultimately avoid deforestation""; ""Recent evidence shows that REDD+ projects have been effective in some regions but efforts are not always sustained over the long term, and a range of barriers exists in other regions""; "The financial resource allocated to environmentally harmful subsidies in various sectors outweighs the resources allocated to biodiversity conservation by a factor of 10 to 1."; "Fast and bold actions are needed to eliminate harmful subsidies to halt biodiversity loss and to mitigate climate change simultaneously."; </t>
-  </si>
-  <si>
-    <t>""Restoration programs provide opportunities for climate change mitigation and biodiversity conservation by recovering degraded ecosystems.""; REDD+ projects aim to align national climate change mitigation and biodiversity goals, slowing deforestation and protecting carbon-rich ecosystems""; ""Wetlands and intact inland ecosystems regulate hazards such as flooding and provide resilience against extreme weather events."";  ""Protected areas in coastal and marine ecosystems enhance cultural and recreational benefits through conservation and sustainable tourism.""; ""The post-2020 Global Biodiversity Framework includes targets that emphasize the contributions of Indigenous Peoples and Local Communities (IPLCs).""; ""Restoration and conservation programs safeguard ecosystem resilience and options for future biodiversity benefits.""; "Implementing a well-connected and effective system of protected areas supports the resilience of biodiversity and provides continued ecosystem services for people, including water regulation and disaster mitigation."; "Conservation efforts must balance trade-offs between global biodiversity goals and local livelihoods, ensuring that governance frameworks are equitable and inclusive."</t>
   </si>
   <si>
     <t>"REDD+ projects aim to align national climate change mitigation and biodiversity goals, slowing deforestation and protecting carbon-rich ecosystems."; ""Biodiversity offsets can limit local people's access to, or cause loss of benefits from, the biodiversity and nature's contributions to people on which their livelihoods depend.""; "Biodiversity offsetting projects often fail to compensate local communities for lost ecosystem services, leading to trade-offs between conservation and human well-being."; "REDD+ projects have had varying success in balancing carbon sequestration with local economic benefits, as financial sustainability remains a key barrier."</t>
@@ -930,411 +908,414 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BAE76B3-84F4-8A48-995C-3E3829696CA9}">
-  <dimension ref="A1:EB5"/>
+  <dimension ref="A1:EB4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="17" max="17" width="35.546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:132" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:132" ht="68.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>40</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>42</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>43</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="V1" t="s">
         <v>45</v>
       </c>
-      <c r="R1" t="s">
+      <c r="W1" t="s">
         <v>46</v>
       </c>
-      <c r="S1" t="s">
+      <c r="X1" t="s">
         <v>47</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
         <v>48</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Z1" t="s">
         <v>49</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AA1" t="s">
         <v>50</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AB1" t="s">
         <v>51</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AC1" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AD1" t="s">
         <v>53</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AE1" t="s">
         <v>54</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AF1" t="s">
         <v>55</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AG1" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AH1" t="s">
         <v>57</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AI1" t="s">
         <v>58</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AJ1" t="s">
         <v>59</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AK1" t="s">
         <v>60</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AL1" t="s">
         <v>61</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AM1" t="s">
         <v>62</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AN1" t="s">
         <v>63</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AO1" t="s">
         <v>64</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AP1" t="s">
         <v>65</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AQ1" t="s">
         <v>66</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AR1" t="s">
         <v>67</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AS1" t="s">
         <v>68</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AT1" t="s">
         <v>69</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AU1" t="s">
         <v>70</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AV1" t="s">
         <v>71</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AW1" t="s">
         <v>72</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AX1" t="s">
         <v>73</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AY1" t="s">
         <v>74</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AZ1" t="s">
         <v>75</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BA1" t="s">
         <v>76</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BB1" t="s">
         <v>77</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BC1" t="s">
         <v>78</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BD1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BE1" t="s">
         <v>80</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BF1" t="s">
         <v>81</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BG1" t="s">
         <v>82</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BH1" t="s">
         <v>83</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BI1" t="s">
         <v>84</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BJ1" t="s">
         <v>85</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BK1" t="s">
         <v>86</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BL1" t="s">
         <v>87</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BM1" t="s">
         <v>88</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BN1" t="s">
         <v>89</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BO1" t="s">
         <v>90</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BP1" t="s">
         <v>91</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BQ1" t="s">
         <v>92</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BR1" t="s">
         <v>93</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BS1" t="s">
         <v>94</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BT1" t="s">
         <v>95</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BU1" t="s">
         <v>96</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BV1" t="s">
         <v>97</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BW1" t="s">
         <v>98</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BX1" t="s">
         <v>99</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BY1" t="s">
         <v>100</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BZ1" t="s">
         <v>101</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="CA1" t="s">
         <v>102</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="CB1" t="s">
         <v>103</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CC1" t="s">
         <v>104</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CD1" t="s">
         <v>105</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CE1" t="s">
         <v>106</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CF1" t="s">
         <v>107</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CG1" t="s">
         <v>108</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CH1" t="s">
         <v>109</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CI1" t="s">
         <v>110</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CJ1" t="s">
         <v>111</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CK1" t="s">
         <v>112</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CL1" t="s">
         <v>113</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CM1" t="s">
         <v>114</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CN1" t="s">
         <v>115</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CO1" t="s">
         <v>116</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CP1" t="s">
         <v>117</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CQ1" t="s">
         <v>118</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CR1" t="s">
         <v>119</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CS1" t="s">
         <v>120</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>121</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>122</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>123</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>124</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>125</v>
       </c>
       <c r="CT1" t="s">
         <v>8</v>
       </c>
       <c r="CU1" t="s">
+        <v>121</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>122</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>123</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>125</v>
+      </c>
+      <c r="CZ1" t="s">
         <v>126</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="DA1" t="s">
         <v>127</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="DB1" t="s">
         <v>128</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="DC1" t="s">
         <v>129</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="DD1" t="s">
         <v>130</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DE1" t="s">
         <v>131</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DF1" t="s">
         <v>132</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DG1" t="s">
         <v>133</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DH1" t="s">
         <v>134</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DI1" t="s">
         <v>135</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DJ1" t="s">
         <v>136</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DK1" t="s">
         <v>137</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DL1" t="s">
         <v>138</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DM1" t="s">
         <v>139</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DN1" t="s">
         <v>140</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DO1" t="s">
         <v>141</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="DP1" t="s">
         <v>142</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="DQ1" t="s">
         <v>143</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="DR1" t="s">
         <v>144</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="DS1" t="s">
         <v>145</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="DT1" t="s">
         <v>146</v>
       </c>
-      <c r="DP1" t="s">
+      <c r="DU1" t="s">
         <v>147</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="DV1" t="s">
         <v>148</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="DW1" t="s">
         <v>149</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="DX1" t="s">
         <v>150</v>
       </c>
-      <c r="DT1" t="s">
+      <c r="DY1" t="s">
         <v>151</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="DZ1" t="s">
         <v>152</v>
       </c>
-      <c r="DV1" t="s">
+      <c r="EA1" t="s">
         <v>153</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="EB1" t="s">
         <v>154</v>
       </c>
-      <c r="DX1" t="s">
-        <v>155</v>
-      </c>
-      <c r="DY1" t="s">
-        <v>156</v>
-      </c>
-      <c r="DZ1" t="s">
-        <v>157</v>
-      </c>
-      <c r="EA1" t="s">
-        <v>158</v>
-      </c>
-      <c r="EB1" t="s">
-        <v>159</v>
-      </c>
     </row>
-    <row r="2" spans="1:132" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:132" ht="409.5" x14ac:dyDescent="0.6">
       <c r="A2">
         <v>76</v>
       </c>
@@ -1381,148 +1362,148 @@
         <v>8</v>
       </c>
       <c r="Q2" t="s">
+        <v>155</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="S2" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" t="s">
         <v>10</v>
       </c>
-      <c r="S2" t="s">
-        <v>11</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
+        <v>159</v>
+      </c>
+      <c r="V2" t="s">
+        <v>11</v>
+      </c>
+      <c r="W2" t="s">
         <v>12</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AH2" t="s">
         <v>13</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AJ2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN2" t="s">
         <v>14</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AT2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB2" t="s">
         <v>15</v>
       </c>
-      <c r="X2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG2" s="2" t="s">
+      <c r="BE2" t="s">
+        <v>11</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>11</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>11</v>
+      </c>
+      <c r="BQ2" t="s">
         <v>16</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="BS2" t="s">
+        <v>11</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>11</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>11</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>11</v>
+      </c>
+      <c r="BX2" t="s">
         <v>17</v>
       </c>
-      <c r="AJ2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AN2" t="s">
+      <c r="BY2" t="s">
+        <v>164</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>12</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>12</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>11</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>11</v>
+      </c>
+      <c r="CG2" t="s">
         <v>19</v>
       </c>
-      <c r="AT2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>14</v>
-      </c>
-      <c r="BB2" t="s">
+      <c r="CH2" t="s">
         <v>20</v>
       </c>
-      <c r="BE2" t="s">
-        <v>14</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>14</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>14</v>
-      </c>
-      <c r="BQ2" t="s">
+      <c r="CI2" t="s">
         <v>21</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>14</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>14</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>14</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>14</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>169</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>15</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>15</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>14</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>14</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>24</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>25</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>26</v>
       </c>
       <c r="CJ2" t="s">
         <v>3</v>
       </c>
       <c r="CK2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="CL2" t="s">
         <v>6</v>
       </c>
       <c r="CM2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="CN2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="CQ2" t="b">
         <v>0</v>
@@ -1639,7 +1620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:132" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:132" ht="409.5" x14ac:dyDescent="0.6">
       <c r="A3">
         <v>76</v>
       </c>
@@ -1686,148 +1667,148 @@
         <v>8</v>
       </c>
       <c r="Q3" t="s">
+        <v>156</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="S3" t="s">
+        <v>9</v>
+      </c>
+      <c r="T3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" t="s">
         <v>160</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="S3" t="s">
-        <v>11</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
+        <v>11</v>
+      </c>
+      <c r="W3" t="s">
         <v>12</v>
       </c>
-      <c r="U3" t="s">
-        <v>164</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN3" t="s">
         <v>14</v>
       </c>
-      <c r="W3" t="s">
+      <c r="AT3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB3" t="s">
         <v>15</v>
       </c>
-      <c r="X3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AH3" t="s">
+      <c r="BE3" t="s">
+        <v>11</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>11</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>11</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>16</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>11</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>11</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>11</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>11</v>
+      </c>
+      <c r="BX3" t="s">
         <v>17</v>
       </c>
-      <c r="AJ3" t="s">
-        <v>167</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AN3" t="s">
+      <c r="BY3" t="s">
+        <v>18</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>12</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>12</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>11</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>11</v>
+      </c>
+      <c r="CG3" t="s">
         <v>19</v>
       </c>
-      <c r="AT3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>14</v>
-      </c>
-      <c r="BB3" t="s">
+      <c r="CH3" t="s">
         <v>20</v>
       </c>
-      <c r="BE3" t="s">
-        <v>14</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>14</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>14</v>
-      </c>
-      <c r="BQ3" t="s">
+      <c r="CI3" t="s">
         <v>21</v>
-      </c>
-      <c r="BS3" t="s">
-        <v>14</v>
-      </c>
-      <c r="BT3" t="s">
-        <v>14</v>
-      </c>
-      <c r="BU3" t="s">
-        <v>14</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>14</v>
-      </c>
-      <c r="BX3" t="s">
-        <v>22</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>170</v>
-      </c>
-      <c r="CB3" t="s">
-        <v>15</v>
-      </c>
-      <c r="CC3" t="s">
-        <v>15</v>
-      </c>
-      <c r="CD3" t="s">
-        <v>14</v>
-      </c>
-      <c r="CE3" t="s">
-        <v>14</v>
-      </c>
-      <c r="CG3" t="s">
-        <v>24</v>
-      </c>
-      <c r="CH3" t="s">
-        <v>25</v>
-      </c>
-      <c r="CI3" t="s">
-        <v>26</v>
       </c>
       <c r="CJ3" t="s">
         <v>3</v>
       </c>
       <c r="CK3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="CL3" t="s">
         <v>6</v>
       </c>
       <c r="CM3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="CN3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="CQ3" t="b">
         <v>0</v>
@@ -1944,313 +1925,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:132" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>76</v>
-      </c>
-      <c r="B4">
-        <v>76</v>
-      </c>
-      <c r="C4">
-        <v>74</v>
-      </c>
-      <c r="D4">
-        <v>148</v>
-      </c>
-      <c r="E4" s="1">
-        <v>45639.590312499997</v>
-      </c>
-      <c r="F4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" t="s">
-        <v>5</v>
-      </c>
-      <c r="N4" t="s">
-        <v>6</v>
-      </c>
-      <c r="O4" t="s">
-        <v>7</v>
-      </c>
-      <c r="P4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>161</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="S4" t="s">
-        <v>11</v>
-      </c>
-      <c r="T4" t="s">
-        <v>12</v>
-      </c>
-      <c r="U4" t="s">
-        <v>165</v>
-      </c>
-      <c r="V4" t="s">
-        <v>14</v>
-      </c>
-      <c r="W4" t="s">
-        <v>15</v>
-      </c>
-      <c r="X4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>168</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>14</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>20</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>14</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>14</v>
-      </c>
-      <c r="BM4" t="s">
-        <v>14</v>
-      </c>
-      <c r="BQ4" t="s">
-        <v>21</v>
-      </c>
-      <c r="BS4" t="s">
-        <v>14</v>
-      </c>
-      <c r="BT4" t="s">
-        <v>14</v>
-      </c>
-      <c r="BU4" t="s">
-        <v>14</v>
-      </c>
-      <c r="BV4" t="s">
-        <v>14</v>
-      </c>
-      <c r="BX4" t="s">
-        <v>22</v>
-      </c>
-      <c r="BY4" t="s">
-        <v>23</v>
-      </c>
-      <c r="CB4" t="s">
-        <v>15</v>
-      </c>
-      <c r="CC4" t="s">
-        <v>15</v>
-      </c>
-      <c r="CD4" t="s">
-        <v>14</v>
-      </c>
-      <c r="CE4" t="s">
-        <v>14</v>
-      </c>
-      <c r="CG4" t="s">
-        <v>24</v>
-      </c>
-      <c r="CH4" t="s">
-        <v>25</v>
-      </c>
-      <c r="CI4" t="s">
-        <v>26</v>
-      </c>
-      <c r="CJ4" t="s">
-        <v>3</v>
-      </c>
-      <c r="CK4" t="s">
-        <v>27</v>
-      </c>
-      <c r="CL4" t="s">
-        <v>6</v>
-      </c>
-      <c r="CM4" t="s">
-        <v>28</v>
-      </c>
-      <c r="CN4" t="s">
-        <v>29</v>
-      </c>
-      <c r="CQ4" t="b">
-        <v>0</v>
-      </c>
-      <c r="CR4" t="b">
-        <v>0</v>
-      </c>
-      <c r="CS4" t="b">
-        <v>0</v>
-      </c>
-      <c r="CT4" t="b">
-        <v>1</v>
-      </c>
-      <c r="CU4" t="b">
-        <v>0</v>
-      </c>
-      <c r="CV4">
-        <v>1</v>
-      </c>
-      <c r="CW4">
-        <v>74</v>
-      </c>
-      <c r="CX4">
-        <v>76</v>
-      </c>
-      <c r="CY4" t="b">
-        <v>1</v>
-      </c>
-      <c r="CZ4" t="b">
-        <v>1</v>
-      </c>
-      <c r="DA4" t="b">
-        <v>1</v>
-      </c>
-      <c r="DB4" t="b">
-        <v>1</v>
-      </c>
-      <c r="DC4" t="b">
-        <v>1</v>
-      </c>
-      <c r="DD4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DE4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DF4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DG4" t="b">
-        <v>1</v>
-      </c>
-      <c r="DH4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DI4" t="b">
-        <v>1</v>
-      </c>
-      <c r="DJ4" t="b">
-        <v>1</v>
-      </c>
-      <c r="DK4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DL4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DM4" t="b">
-        <v>1</v>
-      </c>
-      <c r="DN4" t="b">
-        <v>1</v>
-      </c>
-      <c r="DO4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DP4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DQ4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DR4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DS4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DT4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DU4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DV4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DW4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DX4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DY4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DZ4" t="b">
-        <v>0</v>
-      </c>
-      <c r="EA4" t="b">
-        <v>0</v>
-      </c>
-      <c r="EB4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:132" x14ac:dyDescent="0.2">
-      <c r="E5" s="1"/>
+    <row r="4" spans="1:132" x14ac:dyDescent="0.6">
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>